<commit_message>
code is final for munge??
</commit_message>
<xml_diff>
--- a/raw_ts_data/fd/fd12_ts1.xlsx
+++ b/raw_ts_data/fd/fd12_ts1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncw02\Downloads\IGEA\raw_ts_data\fd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7AF372-7981-4CA5-850F-AF3DF622ED3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DDE01D-82DE-4365-B2A6-812418E18267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A5253AB-7991-5C42-B2D2-1B4C073D839F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2790" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2797" uniqueCount="95">
   <si>
     <t>Reach</t>
   </si>
@@ -317,12 +317,18 @@
   <si>
     <t>EP16</t>
   </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>manual, DEEP SNOW</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -356,6 +362,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -411,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -439,6 +452,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,8 +773,8 @@
   <dimension ref="A1:AC1372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I164" sqref="I164:I179"/>
+      <pane ySplit="1" topLeftCell="A385" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G388" sqref="G388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.21875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8955,7 +8969,7 @@
         <v>47</v>
       </c>
       <c r="C395" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D395" s="1">
         <v>142</v>
@@ -8965,6 +8979,9 @@
       </c>
       <c r="F395" s="1">
         <v>1</v>
+      </c>
+      <c r="G395" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="396" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
@@ -8972,7 +8989,7 @@
         <v>47</v>
       </c>
       <c r="C396" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D396" s="1">
         <v>143</v>
@@ -8982,6 +8999,9 @@
       </c>
       <c r="F396" s="1">
         <v>1</v>
+      </c>
+      <c r="G396" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="397" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
@@ -8989,7 +9009,7 @@
         <v>47</v>
       </c>
       <c r="C397" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D397" s="1">
         <v>144</v>
@@ -8999,6 +9019,9 @@
       </c>
       <c r="F397" s="1">
         <v>1</v>
+      </c>
+      <c r="G397" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="398" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
@@ -9006,7 +9029,7 @@
         <v>47</v>
       </c>
       <c r="C398" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D398" s="1">
         <v>145</v>
@@ -9016,6 +9039,9 @@
       </c>
       <c r="F398" s="1">
         <v>1</v>
+      </c>
+      <c r="G398" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="399" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
@@ -9023,7 +9049,7 @@
         <v>47</v>
       </c>
       <c r="C399" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D399" s="1">
         <v>146</v>
@@ -9034,8 +9060,8 @@
       <c r="F399" s="1">
         <v>3</v>
       </c>
-      <c r="G399" s="1" t="s">
-        <v>51</v>
+      <c r="G399" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="H399" s="1">
         <v>8</v>
@@ -9046,7 +9072,7 @@
         <v>47</v>
       </c>
       <c r="C400" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D400" s="1">
         <v>147</v>
@@ -9056,6 +9082,9 @@
       </c>
       <c r="F400" s="1">
         <v>1</v>
+      </c>
+      <c r="G400" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="401" spans="2:9" ht="13.8" x14ac:dyDescent="0.3">
@@ -9063,7 +9092,7 @@
         <v>47</v>
       </c>
       <c r="C401" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D401" s="1">
         <v>148</v>
@@ -9073,6 +9102,9 @@
       </c>
       <c r="F401" s="1">
         <v>1</v>
+      </c>
+      <c r="G401" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="402" spans="2:9" ht="13.8" x14ac:dyDescent="0.3">
@@ -9080,7 +9112,7 @@
         <v>47</v>
       </c>
       <c r="C402" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D402" s="1">
         <v>149</v>
@@ -9090,6 +9122,9 @@
       </c>
       <c r="F402" s="1">
         <v>1</v>
+      </c>
+      <c r="G402" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="403" spans="2:9" ht="13.8" x14ac:dyDescent="0.3">

</xml_diff>